<commit_message>
Fix update proprietaire montants in av validation issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>512/CASA 2</v>
+        <v>001/TEST DR/AV</v>
       </c>
       <c r="B2" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>31451</v>
+        <v>113564</v>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve">STE LOCATION </v>
+        <v>lala morale</v>
       </c>
       <c r="E2" t="str">
         <v>oui</v>
@@ -440,11 +440,11 @@
       <c r="F2" t="str">
         <v>mensuelle</v>
       </c>
-      <c r="G2">
-        <v>5000</v>
+      <c r="G2" t="str">
+        <v>--</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -456,220 +456,56 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="M2">
-        <v>5000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>512/CASA 2</v>
+        <v>001/TEST DR/AV</v>
       </c>
       <c r="B3" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>56987</v>
+        <v>BB125874</v>
       </c>
       <c r="D3" t="str">
-        <v xml:space="preserve">STE MAISON </v>
+        <v>YASSINE TYEST</v>
       </c>
       <c r="E3" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F3" t="str">
         <v>mensuelle</v>
       </c>
-      <c r="G3">
-        <v>5000</v>
+      <c r="G3" t="str">
+        <v>--</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>36000</v>
       </c>
       <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>36000</v>
       </c>
       <c r="M3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>903/CASA ANFA/AV</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C4" t="str">
-        <v>654566</v>
-      </c>
-      <c r="D4" t="str">
-        <v>STT22</v>
-      </c>
-      <c r="E4" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G4" t="str">
-        <v>--</v>
-      </c>
-      <c r="H4">
-        <v>15000</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>15000</v>
-      </c>
-      <c r="M4">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>602/CASA 2MARS</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C5" t="str">
-        <v>F354654</v>
-      </c>
-      <c r="D5" t="str">
-        <v>SARA DADA</v>
-      </c>
-      <c r="E5" t="str">
-        <v>non</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>40000</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>15</v>
-      </c>
-      <c r="J5">
-        <v>3000</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>20000</v>
-      </c>
-      <c r="M5">
-        <v>37000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>120/SUP 2/AV</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C6" t="str">
-        <v>O3546845</v>
-      </c>
-      <c r="D6" t="str">
-        <v xml:space="preserve">KHALID VAVA </v>
-      </c>
-      <c r="E6" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>9000</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>9000</v>
-      </c>
-      <c r="M6">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>120/SUP 2/AV</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C7" t="str">
-        <v>F6546856</v>
-      </c>
-      <c r="D7" t="str">
-        <v>KARIMA NANA</v>
-      </c>
-      <c r="E7" t="str">
-        <v>non</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7">
-        <v>6000</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-      <c r="J7">
-        <v>600</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>6000</v>
-      </c>
-      <c r="M7">
-        <v>5400</v>
+        <v>66600</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix suspendu mail content issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -790,9 +790,50 @@
         <v>66600</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>569/SUP 9999</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Supervision</v>
+      </c>
+      <c r="C11" t="str">
+        <v>KL365695</v>
+      </c>
+      <c r="D11" t="str">
+        <v xml:space="preserve">YAYA TATA </v>
+      </c>
+      <c r="E11" t="str">
+        <v>non</v>
+      </c>
+      <c r="F11" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G11">
+        <v>80000</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>12000</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>68000</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix résilie mail content issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -790,50 +790,9 @@
         <v>66600</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>569/SUP 9999</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C11" t="str">
-        <v>KL365695</v>
-      </c>
-      <c r="D11" t="str">
-        <v xml:space="preserve">YAYA TATA </v>
-      </c>
-      <c r="E11" t="str">
-        <v>non</v>
-      </c>
-      <c r="F11" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G11">
-        <v>80000</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>15</v>
-      </c>
-      <c r="J11">
-        <v>12000</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>68000</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Populate contrat by id with the old contrat
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -400,13 +400,13 @@
         <v>Périodicité</v>
       </c>
       <c r="G1" t="str">
+        <v>Taux de taxe</v>
+      </c>
+      <c r="H1" t="str">
         <v>MT brut de loyer</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>MT brut d'avance</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Taux de taxe</v>
       </c>
       <c r="J1" t="str">
         <v>Taxe/loyer</v>
@@ -423,57 +423,57 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>903/CASA ANFA/AV</v>
+        <v>001/DR TANGER</v>
       </c>
       <c r="B2" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>654566</v>
+        <v>bj123465</v>
       </c>
       <c r="D2" t="str">
-        <v>STT22</v>
+        <v>Test Tse</v>
       </c>
       <c r="E2" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F2" t="str">
         <v>mensuelle</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2" t="str">
         <v>--</v>
       </c>
-      <c r="H2">
-        <v>15000</v>
-      </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
+        <v>60000</v>
+      </c>
+      <c r="J2" t="str">
+        <v>--</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>9000</v>
       </c>
       <c r="L2">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="M2">
-        <v>15000</v>
+        <v>71000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>965/PVFF222/AV</v>
+        <v>006/123</v>
       </c>
       <c r="B3" t="str">
-        <v>Point de vente</v>
+        <v>Siège</v>
       </c>
       <c r="C3" t="str">
-        <v>L3546465</v>
+        <v>BJ12348</v>
       </c>
       <c r="D3" t="str">
-        <v>ZAZA EELA</v>
+        <v>Ahmed laaraichi</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -482,317 +482,71 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>6000</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="H3" t="str">
+        <v>--</v>
       </c>
       <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>600</v>
+        <v>90000</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>13500</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="M3">
-        <v>5400</v>
+        <v>166500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>965/PVFF222/AV</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B4" t="str">
-        <v>Point de vente</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C4" t="str">
-        <v>K5346431</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D4" t="str">
-        <v>SARA ELLLL</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E4" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G4">
-        <v>14000</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G4" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>150000</v>
       </c>
       <c r="J4">
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>22500</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>110000</v>
       </c>
       <c r="M4">
-        <v>11900</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>662/PV 55586/AV</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C5" t="str">
-        <v>354653</v>
-      </c>
-      <c r="D5" t="str">
-        <v>STE 663</v>
-      </c>
-      <c r="E5" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>5000</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>662/PV 55586/AV</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C6" t="str">
-        <v>H6356525</v>
-      </c>
-      <c r="D6" t="str">
-        <v>AVENT LLLL</v>
-      </c>
-      <c r="E6" t="str">
-        <v>non</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>5000</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>500</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>788/SUPP600/AV</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C7" t="str">
-        <v>3546546</v>
-      </c>
-      <c r="D7" t="str">
-        <v>LOCATION 55</v>
-      </c>
-      <c r="E7" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7" t="str">
-        <v>--</v>
-      </c>
-      <c r="H7">
-        <v>10000</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>788/SUPP600/AV</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C8" t="str">
-        <v>35486464</v>
-      </c>
-      <c r="D8" t="str">
-        <v>KJIKHIUHI</v>
-      </c>
-      <c r="E8" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F8" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G8" t="str">
-        <v>--</v>
-      </c>
-      <c r="H8">
-        <v>10000</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>668/TANGER/AV</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C9" t="str">
-        <v>J5498456</v>
-      </c>
-      <c r="D9" t="str">
-        <v>MORAD FFFF</v>
-      </c>
-      <c r="E9" t="str">
-        <v>non</v>
-      </c>
-      <c r="F9" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G9">
-        <v>48000</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>15</v>
-      </c>
-      <c r="J9">
-        <v>3600</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>24000</v>
-      </c>
-      <c r="M9">
-        <v>44400</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>668/TANGER/AV</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C10" t="str">
-        <v>J5648645</v>
-      </c>
-      <c r="D10" t="str">
-        <v>SALMA KJLJOIO</v>
-      </c>
-      <c r="E10" t="str">
-        <v>non</v>
-      </c>
-      <c r="F10" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G10">
-        <v>72000</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>15</v>
-      </c>
-      <c r="J10">
-        <v>5400</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>36000</v>
-      </c>
-      <c r="M10">
-        <v>66600</v>
+        <v>237500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add activate contrat after suspension
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>001/DR TANGER</v>
+        <v>797/DR TADLA</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>bj123465</v>
+        <v>ad646456</v>
       </c>
       <c r="D2" t="str">
-        <v>Test Tse</v>
+        <v>Mimo crimo</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -441,39 +441,39 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H2" t="str">
         <v>--</v>
       </c>
       <c r="I2">
-        <v>60000</v>
+        <v>6000</v>
       </c>
       <c r="J2" t="str">
         <v>--</v>
       </c>
       <c r="K2">
-        <v>9000</v>
+        <v>600</v>
       </c>
       <c r="L2">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>71000</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>006/123</v>
+        <v>010/DR010/AV</v>
       </c>
       <c r="B3" t="str">
-        <v>Siège</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>BJ12348</v>
+        <v>aa654556</v>
       </c>
       <c r="D3" t="str">
-        <v>Ahmed laaraichi</v>
+        <v>Ali Ali</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -482,71 +482,194 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H3" t="str">
         <v>--</v>
       </c>
       <c r="I3">
-        <v>90000</v>
-      </c>
-      <c r="J3" t="str">
-        <v>--</v>
+        <v>2000</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>13500</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>166500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
+        <v>001/DR TANGER/AV</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C4" t="str">
+        <v>ada666</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Mohamed berrada</v>
+      </c>
+      <c r="E4" t="str">
+        <v>non</v>
+      </c>
+      <c r="F4" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4" t="str">
+        <v>--</v>
+      </c>
+      <c r="I4">
+        <v>5000</v>
+      </c>
+      <c r="J4" t="str">
+        <v>--</v>
+      </c>
+      <c r="K4">
+        <v>500</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>000/DR DEV</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C5" t="str">
+        <v>117946464</v>
+      </c>
+      <c r="D5" t="str">
+        <v>IBM</v>
+      </c>
+      <c r="E5" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F5" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>30000</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>20000</v>
+      </c>
+      <c r="M5">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>000/DR DEV</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C6" t="str">
+        <v>BJ179134</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Ahmed Tawfiq</v>
+      </c>
+      <c r="E6" t="str">
+        <v>non</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>30000</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1500</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>20000</v>
+      </c>
+      <c r="M6">
+        <v>28500</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B4" t="str">
+      <c r="B7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C4" t="str">
+      <c r="C7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D4" t="str">
+      <c r="D7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E4" t="str">
+      <c r="E7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F4" t="str">
+      <c r="F7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G4" t="str">
+      <c r="G7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>150000</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>22500</v>
-      </c>
-      <c r="L4">
-        <v>110000</v>
-      </c>
-      <c r="M4">
-        <v>237500</v>
+      <c r="H7">
+        <v>60000</v>
+      </c>
+      <c r="I7">
+        <v>13000</v>
+      </c>
+      <c r="J7">
+        <v>1500</v>
+      </c>
+      <c r="K7">
+        <v>1100</v>
+      </c>
+      <c r="L7">
+        <v>40000</v>
+      </c>
+      <c r="M7">
+        <v>70400</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix avenent issues :
- Duplecate proprietaire into new contrat
- Recalculate montants proprietaire
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_4_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,253 +423,48 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>797/DR TADLA</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B2" t="str">
-        <v>Direction régionale</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <v>ad646456</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D2" t="str">
-        <v>Mimo crimo</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E2" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F2" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2" t="str">
-        <v>--</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G2" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>6000</v>
-      </c>
-      <c r="J2" t="str">
-        <v>--</v>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>010/DR010/AV</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C3" t="str">
-        <v>aa654556</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Ali Ali</v>
-      </c>
-      <c r="E3" t="str">
-        <v>non</v>
-      </c>
-      <c r="F3" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="str">
-        <v>--</v>
-      </c>
-      <c r="I3">
-        <v>2000</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>001/DR TANGER/AV</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C4" t="str">
-        <v>ada666</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Mohamed berrada</v>
-      </c>
-      <c r="E4" t="str">
-        <v>non</v>
-      </c>
-      <c r="F4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4" t="str">
-        <v>--</v>
-      </c>
-      <c r="I4">
-        <v>5000</v>
-      </c>
-      <c r="J4" t="str">
-        <v>--</v>
-      </c>
-      <c r="K4">
-        <v>500</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>000/DR DEV</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C5" t="str">
-        <v>117946464</v>
-      </c>
-      <c r="D5" t="str">
-        <v>IBM</v>
-      </c>
-      <c r="E5" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>30000</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>20000</v>
-      </c>
-      <c r="M5">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>000/DR DEV</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C6" t="str">
-        <v>BJ179134</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Ahmed Tawfiq</v>
-      </c>
-      <c r="E6" t="str">
-        <v>non</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>15</v>
-      </c>
-      <c r="H6">
-        <v>30000</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>1500</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>20000</v>
-      </c>
-      <c r="M6">
-        <v>28500</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H7">
-        <v>60000</v>
-      </c>
-      <c r="I7">
-        <v>13000</v>
-      </c>
-      <c r="J7">
-        <v>1500</v>
-      </c>
-      <c r="K7">
-        <v>1100</v>
-      </c>
-      <c r="L7">
-        <v>40000</v>
-      </c>
-      <c r="M7">
-        <v>70400</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>